<commit_message>
Update Budget and Timeline
</commit_message>
<xml_diff>
--- a/Logistics/Budget.xlsx
+++ b/Logistics/Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Google Drive\495 project\Timeline and Budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\SeniorDesign\Logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>3 wire 20 gauge power cable 10'</t>
-  </si>
-  <si>
-    <t>ViewSonic PJD5134 SVGA DLP Projector</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/ViewSonic-PJD5134-Projector-Lumens-Blu-Ray/dp/B00A9S3OOC/ref=sr_1_5?ie=UTF8&amp;qid=1395978933&amp;sr=8-5&amp;keywords=business+projector</t>
   </si>
   <si>
     <t>Imaging</t>
@@ -586,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T108"/>
+  <dimension ref="A1:T107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -645,23 +639,23 @@
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:D13" si="0">(B2*C2)</f>
-        <v>30</v>
+        <f t="shared" ref="D2:D10" si="0">(B2*C2)</f>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -682,23 +676,23 @@
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5">
-        <v>1.34</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>1.34</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
@@ -718,24 +712,24 @@
       <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6">
-        <v>6.95</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <v>21.56</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>6.95</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>86.24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -756,20 +750,20 @@
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5">
-        <v>45</v>
+        <v>46.85</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>93.7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -793,26 +787,26 @@
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
-        <v>17.100000000000001</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>17.100000000000001</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="7"/>
@@ -830,20 +824,20 @@
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5">
-        <v>21.56</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>86.24</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -867,26 +861,26 @@
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5">
-        <v>46.85</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>93.7</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="7"/>
@@ -904,26 +898,26 @@
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="7"/>
@@ -941,25 +935,23 @@
     </row>
     <row r="10" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="3"/>
@@ -978,25 +970,24 @@
     </row>
     <row r="11" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="3"/>
@@ -1015,26 +1006,26 @@
     </row>
     <row r="12" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B12" s="5">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>148</v>
+        <f t="shared" ref="D12:D23" si="1">(B12*C12)</f>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="7"/>
@@ -1052,23 +1043,25 @@
     </row>
     <row r="13" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E13" s="3"/>
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="3"/>
@@ -1087,25 +1080,26 @@
     </row>
     <row r="14" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B14" s="5">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>34</v>
+        <f>(B14*C14)</f>
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="7"/>
@@ -1123,26 +1117,26 @@
     </row>
     <row r="15" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
-        <v>22</v>
+        <v>1.34</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" ref="D15:D24" si="1">(B15*C15)</f>
-        <v>22</v>
+        <f>(B15*C15)</f>
+        <v>1.34</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="7"/>
@@ -1159,24 +1153,24 @@
       <c r="T15" s="7"/>
     </row>
     <row r="16" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="5">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>6.95</v>
+      </c>
+      <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>41</v>
+        <f>(B16*C16)</f>
+        <v>6.95</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
@@ -1382,23 +1376,23 @@
     </row>
     <row r="22" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="5">
-        <v>329.99</v>
+        <v>2.57</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="1"/>
-        <v>329.99</v>
+        <v>5.14</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>16</v>
@@ -1422,20 +1416,20 @@
         <v>55</v>
       </c>
       <c r="B23" s="5">
-        <v>2.57</v>
+        <v>10.9</v>
       </c>
       <c r="C23" s="3">
         <v>2</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="1"/>
-        <v>5.14</v>
+        <v>21.8</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>56</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>16</v>
@@ -1454,30 +1448,16 @@
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
     </row>
-    <row r="24" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="C24" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="5">
-        <v>10.9</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2</v>
-      </c>
-      <c r="D24" s="5">
-        <f t="shared" si="1"/>
-        <v>21.8</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="3"/>
+      <c r="D24" s="12">
+        <f>SUM(D2:D23)</f>
+        <v>637.48000000000013</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -1491,14 +1471,10 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
     </row>
-    <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.25">
-      <c r="C25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="12">
-        <f>SUM(D2:D24)</f>
-        <v>967.47</v>
-      </c>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="E25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -1514,10 +1490,9 @@
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="E26" s="7"/>
+    <row r="26" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="10"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -1533,7 +1508,7 @@
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
     </row>
-    <row r="27" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -1588,7 +1563,11 @@
       <c r="T29" s="7"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -1609,7 +1588,7 @@
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -3299,28 +3278,6 @@
       <c r="S107" s="7"/>
       <c r="T107" s="7"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A108" s="7"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="7"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-      <c r="J108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="7"/>
-      <c r="M108" s="7"/>
-      <c r="N108" s="7"/>
-      <c r="O108" s="7"/>
-      <c r="P108" s="7"/>
-      <c r="Q108" s="7"/>
-      <c r="R108" s="7"/>
-      <c r="S108" s="7"/>
-      <c r="T108" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>